<commit_message>
Output with updated font and background colors
</commit_message>
<xml_diff>
--- a/output-seating-order.xlsx
+++ b/output-seating-order.xlsx
@@ -29,10 +29,10 @@
       <b val="1"/>
     </font>
     <font>
-      <color rgb="000000FF"/>
+      <color rgb="00008000"/>
     </font>
     <font>
-      <color rgb="00FFFF00"/>
+      <color rgb="000000FF"/>
     </font>
     <font>
       <color rgb="00FF0000"/>
@@ -57,7 +57,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00CED2C2"/>
+        <fgColor rgb="00BBA5FF"/>
       </patternFill>
     </fill>
     <fill>
@@ -89,7 +89,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -101,10 +101,12 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -470,7 +472,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B114"/>
+  <dimension ref="A1:B115"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -843,684 +845,692 @@
       <c r="B39" t="inlineStr"/>
     </row>
     <row r="40">
-      <c r="A40" t="inlineStr"/>
+      <c r="A40" s="2" t="inlineStr">
+        <is>
+          <t>Jouko Mustonen</t>
+        </is>
+      </c>
       <c r="B40" s="2" t="inlineStr">
         <is>
-          <t>Jouko Mustonen</t>
+          <t>Marita Mustonen</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="2" t="inlineStr">
         <is>
-          <t>Marita Mustonen</t>
+          <t>Joni Mustonen</t>
         </is>
       </c>
       <c r="B41" s="2" t="inlineStr">
         <is>
-          <t>Joni Mustonen</t>
+          <t>Anja Mustonen</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="2" t="inlineStr">
         <is>
-          <t>Anja Mustonen</t>
-        </is>
-      </c>
-      <c r="B42" s="2" t="inlineStr">
-        <is>
           <t>Esko Mustonen</t>
         </is>
       </c>
+      <c r="B42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr"/>
       <c r="B43" t="inlineStr"/>
     </row>
     <row r="44">
-      <c r="A44" t="inlineStr"/>
+      <c r="A44" s="3" t="inlineStr">
+        <is>
+          <t>Ilona Peltonen</t>
+        </is>
+      </c>
       <c r="B44" s="3" t="inlineStr">
         <is>
-          <t>Ilona Peltonen</t>
+          <t>Joonas Peltonen</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="3" t="inlineStr">
         <is>
-          <t>Joonas Peltonen</t>
+          <t>Amanda Peltonen</t>
         </is>
       </c>
       <c r="B45" s="3" t="inlineStr">
         <is>
-          <t>Amanda Peltonen</t>
+          <t>Henri Peltonen</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="3" t="inlineStr">
         <is>
-          <t>Henri Peltonen</t>
-        </is>
-      </c>
-      <c r="B46" s="3" t="inlineStr">
-        <is>
           <t>Irene Peltonen</t>
         </is>
       </c>
+      <c r="B46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr"/>
       <c r="B47" t="inlineStr"/>
     </row>
     <row r="48">
-      <c r="A48" t="inlineStr"/>
+      <c r="A48" s="4" t="inlineStr">
+        <is>
+          <t>Kalle Lappalainen</t>
+        </is>
+      </c>
       <c r="B48" s="4" t="inlineStr">
         <is>
-          <t>Kalle Lappalainen</t>
+          <t>Sisko Lappalainen</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="4" t="inlineStr">
         <is>
-          <t>Sisko Lappalainen</t>
+          <t>Ilkka Lappalainen</t>
         </is>
       </c>
       <c r="B49" s="4" t="inlineStr">
         <is>
-          <t>Ilkka Lappalainen</t>
+          <t>Julia Lappalainen</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="4" t="inlineStr">
         <is>
-          <t>Julia Lappalainen</t>
-        </is>
-      </c>
-      <c r="B50" s="4" t="inlineStr">
-        <is>
           <t>Elias Lappalainen</t>
         </is>
       </c>
+      <c r="B50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr"/>
       <c r="B51" t="inlineStr"/>
     </row>
     <row r="52">
-      <c r="A52" t="inlineStr"/>
+      <c r="A52" s="5" t="inlineStr">
+        <is>
+          <t>Eila Koskela</t>
+        </is>
+      </c>
       <c r="B52" s="5" t="inlineStr">
         <is>
-          <t>Eila Koskela</t>
+          <t>Paavo Koskela</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="5" t="inlineStr">
         <is>
-          <t>Paavo Koskela</t>
+          <t>Marianne Koskela</t>
         </is>
       </c>
       <c r="B53" s="5" t="inlineStr">
         <is>
-          <t>Marianne Koskela</t>
+          <t>Pauli Koskela</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="5" t="inlineStr">
         <is>
-          <t>Pauli Koskela</t>
-        </is>
-      </c>
-      <c r="B54" s="5" t="inlineStr">
-        <is>
           <t>Katriina Koskela</t>
         </is>
       </c>
+      <c r="B54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr"/>
       <c r="B55" t="inlineStr"/>
     </row>
     <row r="56">
-      <c r="A56" t="inlineStr"/>
+      <c r="A56" s="6" t="inlineStr">
+        <is>
+          <t>Mikael Huttunen</t>
+        </is>
+      </c>
       <c r="B56" s="6" t="inlineStr">
         <is>
-          <t>Mikael Huttunen</t>
+          <t>Aurora Huttunen</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="6" t="inlineStr">
         <is>
-          <t>Aurora Huttunen</t>
+          <t>Onni Huttunen</t>
         </is>
       </c>
       <c r="B57" s="6" t="inlineStr">
         <is>
-          <t>Onni Huttunen</t>
+          <t>Elisabeth Huttunen</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="6" t="inlineStr">
         <is>
-          <t>Elisabeth Huttunen</t>
-        </is>
-      </c>
-      <c r="B58" s="6" t="inlineStr">
-        <is>
           <t>Tapio Huttunen</t>
         </is>
       </c>
+      <c r="B58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr"/>
       <c r="B59" t="inlineStr"/>
     </row>
     <row r="60">
-      <c r="A60" t="inlineStr"/>
+      <c r="A60" s="2" t="inlineStr">
+        <is>
+          <t>Arja Pesonen</t>
+        </is>
+      </c>
       <c r="B60" s="2" t="inlineStr">
         <is>
-          <t>Arja Pesonen</t>
+          <t>Veli Pesonen</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="2" t="inlineStr">
         <is>
-          <t>Veli Pesonen</t>
+          <t>Marjaana Pesonen</t>
         </is>
       </c>
       <c r="B61" s="2" t="inlineStr">
         <is>
-          <t>Marjaana Pesonen</t>
+          <t>Leevi Pesonen</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="2" t="inlineStr">
         <is>
-          <t>Leevi Pesonen</t>
-        </is>
-      </c>
-      <c r="B62" s="2" t="inlineStr">
-        <is>
           <t>Kaisa Pesonen</t>
         </is>
       </c>
+      <c r="B62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr"/>
       <c r="B63" t="inlineStr"/>
     </row>
     <row r="64">
-      <c r="A64" t="inlineStr"/>
+      <c r="A64" s="3" t="inlineStr">
+        <is>
+          <t>Jyrki Johansson</t>
+        </is>
+      </c>
       <c r="B64" s="3" t="inlineStr">
         <is>
-          <t>Jyrki Johansson</t>
+          <t>Marketta Johansson</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="3" t="inlineStr">
         <is>
-          <t>Marketta Johansson</t>
+          <t>Lasse Johansson</t>
         </is>
       </c>
       <c r="B65" s="3" t="inlineStr">
         <is>
-          <t>Lasse Johansson</t>
+          <t>Elisa Johansson</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="3" t="inlineStr">
         <is>
-          <t>Elisa Johansson</t>
-        </is>
-      </c>
-      <c r="B66" s="3" t="inlineStr">
-        <is>
           <t>Aki Johansson</t>
         </is>
       </c>
+      <c r="B66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr"/>
       <c r="B67" t="inlineStr"/>
     </row>
     <row r="68">
-      <c r="A68" t="inlineStr"/>
+      <c r="A68" s="4" t="inlineStr">
+        <is>
+          <t>Terttu Vainio</t>
+        </is>
+      </c>
       <c r="B68" s="4" t="inlineStr">
         <is>
-          <t>Terttu Vainio</t>
+          <t>Juhani Vainio</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="4" t="inlineStr">
         <is>
-          <t>Juhani Vainio</t>
+          <t>Jenni Vainio</t>
         </is>
       </c>
       <c r="B69" s="4" t="inlineStr">
         <is>
-          <t>Jenni Vainio</t>
+          <t>Riku Vainio</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="4" t="inlineStr">
         <is>
-          <t>Riku Vainio</t>
-        </is>
-      </c>
-      <c r="B70" s="4" t="inlineStr">
-        <is>
           <t>Emma Vainio</t>
         </is>
       </c>
+      <c r="B70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr"/>
       <c r="B71" t="inlineStr"/>
     </row>
     <row r="72">
-      <c r="A72" t="inlineStr"/>
+      <c r="A72" s="5" t="inlineStr">
+        <is>
+          <t>Otto Immonen</t>
+        </is>
+      </c>
       <c r="B72" s="5" t="inlineStr">
         <is>
-          <t>Otto Immonen</t>
+          <t>Heli Immonen</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="5" t="inlineStr">
         <is>
-          <t>Heli Immonen</t>
+          <t>Daniel Immonen</t>
         </is>
       </c>
       <c r="B73" s="5" t="inlineStr">
         <is>
-          <t>Daniel Immonen</t>
+          <t>Nina Immonen</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="5" t="inlineStr">
         <is>
-          <t>Nina Immonen</t>
-        </is>
-      </c>
-      <c r="B74" s="5" t="inlineStr">
-        <is>
           <t>Miika Immonen</t>
         </is>
       </c>
+      <c r="B74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr"/>
       <c r="B75" t="inlineStr"/>
     </row>
     <row r="76">
-      <c r="A76" t="inlineStr"/>
+      <c r="A76" s="6" t="inlineStr">
+        <is>
+          <t>Maaria Kokkonen</t>
+        </is>
+      </c>
       <c r="B76" s="6" t="inlineStr">
         <is>
-          <t>Maaria Kokkonen</t>
+          <t>Jarno Kokkonen</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="6" t="inlineStr">
         <is>
-          <t>Jarno Kokkonen</t>
+          <t>Mirja Kokkonen</t>
         </is>
       </c>
       <c r="B77" s="6" t="inlineStr">
         <is>
-          <t>Mirja Kokkonen</t>
+          <t>Valtteri Kokkonen</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="6" t="inlineStr">
         <is>
-          <t>Valtteri Kokkonen</t>
-        </is>
-      </c>
-      <c r="B78" s="6" t="inlineStr">
-        <is>
           <t>Sara Kokkonen</t>
         </is>
       </c>
+      <c r="B78" t="inlineStr"/>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr"/>
       <c r="B79" t="inlineStr"/>
     </row>
     <row r="80">
-      <c r="A80" t="inlineStr"/>
+      <c r="A80" s="2" t="inlineStr">
+        <is>
+          <t>Rasmus Laukkanen</t>
+        </is>
+      </c>
       <c r="B80" s="2" t="inlineStr">
         <is>
-          <t>Rasmus Laukkanen</t>
+          <t>Raili Laukkanen</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="2" t="inlineStr">
         <is>
-          <t>Raili Laukkanen</t>
+          <t>Reino Laukkanen</t>
         </is>
       </c>
       <c r="B81" s="2" t="inlineStr">
         <is>
-          <t>Reino Laukkanen</t>
+          <t>Ella Laukkanen</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="2" t="inlineStr">
         <is>
-          <t>Ella Laukkanen</t>
-        </is>
-      </c>
-      <c r="B82" s="2" t="inlineStr">
-        <is>
           <t>Oliver Laukkanen</t>
         </is>
       </c>
+      <c r="B82" t="inlineStr"/>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr"/>
       <c r="B83" t="inlineStr"/>
     </row>
     <row r="84">
-      <c r="A84" t="inlineStr"/>
+      <c r="A84" s="3" t="inlineStr">
+        <is>
+          <t>Aleksandra Kangas</t>
+        </is>
+      </c>
       <c r="B84" s="3" t="inlineStr">
         <is>
-          <t>Aleksandra Kangas</t>
+          <t>Roope Kangas</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="3" t="inlineStr">
         <is>
-          <t>Roope Kangas</t>
+          <t>Kaija Kangas</t>
         </is>
       </c>
       <c r="B85" s="3" t="inlineStr">
         <is>
-          <t>Kaija Kangas</t>
+          <t>Ossi Kangas</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="3" t="inlineStr">
         <is>
-          <t>Ossi Kangas</t>
-        </is>
-      </c>
-      <c r="B86" s="3" t="inlineStr">
-        <is>
           <t>Marjut Kangas</t>
         </is>
       </c>
+      <c r="B86" t="inlineStr"/>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr"/>
       <c r="B87" t="inlineStr"/>
     </row>
     <row r="88">
-      <c r="A88" t="inlineStr"/>
+      <c r="A88" s="4" t="inlineStr">
+        <is>
+          <t>Olavi Leino</t>
+        </is>
+      </c>
       <c r="B88" s="4" t="inlineStr">
         <is>
-          <t>Olavi Leino</t>
+          <t>Alexandra Leino</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="4" t="inlineStr">
         <is>
-          <t>Alexandra Leino</t>
+          <t>Ismo Leino</t>
         </is>
       </c>
       <c r="B89" s="4" t="inlineStr">
         <is>
-          <t>Ismo Leino</t>
+          <t>Saara Leino</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="4" t="inlineStr">
         <is>
-          <t>Saara Leino</t>
-        </is>
-      </c>
-      <c r="B90" s="4" t="inlineStr">
-        <is>
           <t>Anssi Leino</t>
         </is>
       </c>
+      <c r="B90" t="inlineStr"/>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr"/>
       <c r="B91" t="inlineStr"/>
     </row>
     <row r="92">
-      <c r="A92" t="inlineStr"/>
+      <c r="A92" s="5" t="inlineStr">
+        <is>
+          <t>Pia Martikainen</t>
+        </is>
+      </c>
       <c r="B92" s="5" t="inlineStr">
         <is>
-          <t>Pia Martikainen</t>
+          <t>Veijo Martikainen</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="5" t="inlineStr">
         <is>
-          <t>Veijo Martikainen</t>
+          <t>Lea Martikainen</t>
         </is>
       </c>
       <c r="B93" s="5" t="inlineStr">
         <is>
-          <t>Lea Martikainen</t>
+          <t>Emil Martikainen</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="5" t="inlineStr">
         <is>
-          <t>Emil Martikainen</t>
-        </is>
-      </c>
-      <c r="B94" s="5" t="inlineStr">
-        <is>
           <t>Aila Martikainen</t>
         </is>
       </c>
+      <c r="B94" t="inlineStr"/>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr"/>
       <c r="B95" t="inlineStr"/>
     </row>
     <row r="96">
-      <c r="A96" t="inlineStr"/>
+      <c r="A96" s="6" t="inlineStr">
+        <is>
+          <t>Leila Salmela</t>
+        </is>
+      </c>
       <c r="B96" s="6" t="inlineStr">
         <is>
-          <t>Leila Salmela</t>
+          <t>Osmo Salmela</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="6" t="inlineStr">
         <is>
-          <t>Osmo Salmela</t>
+          <t>Henna Salmela</t>
         </is>
       </c>
       <c r="B97" s="6" t="inlineStr">
         <is>
-          <t>Henna Salmela</t>
+          <t>Lassi Salmela</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="6" t="inlineStr">
         <is>
-          <t>Lassi Salmela</t>
-        </is>
-      </c>
-      <c r="B98" s="6" t="inlineStr">
-        <is>
           <t>Lotta Salmela</t>
         </is>
       </c>
+      <c r="B98" t="inlineStr"/>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr"/>
       <c r="B99" t="inlineStr"/>
     </row>
     <row r="100">
-      <c r="A100" t="inlineStr"/>
+      <c r="A100" s="2" t="inlineStr">
+        <is>
+          <t>Samuel Laurila</t>
+        </is>
+      </c>
       <c r="B100" s="2" t="inlineStr">
         <is>
+          <t>Marjo Laurila</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="2" t="inlineStr">
+        <is>
+          <t>Samu Laurila</t>
+        </is>
+      </c>
+      <c r="B101" s="2" t="inlineStr">
+        <is>
+          <t>Tanja Laurila</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="2" t="inlineStr">
+        <is>
+          <t>Asko Laurila</t>
+        </is>
+      </c>
+      <c r="B102" s="9" t="inlineStr">
+        <is>
+          <t>Julius Kuusisto</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="9" t="inlineStr">
+        <is>
+          <t>Topi Kuusisto</t>
+        </is>
+      </c>
+      <c r="B103" s="10" t="inlineStr">
+        <is>
+          <t>Alina Tamminen</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="11" t="inlineStr">
+        <is>
+          <t>Kim Kuusisto</t>
+        </is>
+      </c>
+      <c r="B104" s="12" t="inlineStr">
+        <is>
+          <t>Elli Tamminen</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="7" t="inlineStr">
+        <is>
+          <t>Kati Kuusisto</t>
+        </is>
+      </c>
+      <c r="B105" s="7" t="inlineStr">
+        <is>
+          <t>Margareta Kuusisto</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="13" t="inlineStr">
+        <is>
+          <t>Johan Tamminen</t>
+        </is>
+      </c>
+      <c r="B106" s="13" t="inlineStr">
+        <is>
+          <t>Konsta Tamminen</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="14" t="inlineStr">
+        <is>
+          <t>Marja-Liisa Tamminen</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr"/>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr"/>
+      <c r="B108" t="inlineStr"/>
+    </row>
+    <row r="109">
+      <c r="A109" s="2" t="inlineStr">
+        <is>
           <t>Akseli Karhu</t>
         </is>
       </c>
-    </row>
-    <row r="101">
-      <c r="A101" t="inlineStr"/>
-      <c r="B101" t="inlineStr"/>
-    </row>
-    <row r="102">
-      <c r="A102" t="inlineStr"/>
-      <c r="B102" s="3" t="inlineStr">
-        <is>
-          <t>Samuel Laurila</t>
-        </is>
-      </c>
-    </row>
-    <row r="103">
-      <c r="A103" s="3" t="inlineStr">
-        <is>
-          <t>Marjo Laurila</t>
-        </is>
-      </c>
-      <c r="B103" s="3" t="inlineStr">
-        <is>
-          <t>Samu Laurila</t>
-        </is>
-      </c>
-    </row>
-    <row r="104">
-      <c r="A104" s="3" t="inlineStr">
-        <is>
-          <t>Tanja Laurila</t>
-        </is>
-      </c>
-      <c r="B104" s="3" t="inlineStr">
-        <is>
-          <t>Asko Laurila</t>
-        </is>
-      </c>
-    </row>
-    <row r="105">
-      <c r="A105" s="9" t="inlineStr">
-        <is>
-          <t>Julius Kuusisto</t>
-        </is>
-      </c>
-      <c r="B105" s="9" t="inlineStr">
-        <is>
-          <t>Topi Kuusisto</t>
-        </is>
-      </c>
-    </row>
-    <row r="106">
-      <c r="A106" s="10" t="inlineStr">
-        <is>
-          <t>Kim Kuusisto</t>
-        </is>
-      </c>
-      <c r="B106" s="4" t="inlineStr">
-        <is>
-          <t>Kati Kuusisto</t>
-        </is>
-      </c>
-    </row>
-    <row r="107">
-      <c r="A107" s="4" t="inlineStr">
-        <is>
-          <t>Margareta Kuusisto</t>
-        </is>
-      </c>
-      <c r="B107" s="8" t="inlineStr">
-        <is>
-          <t>Alina Tamminen</t>
-        </is>
-      </c>
-    </row>
-    <row r="108">
-      <c r="A108" s="6" t="inlineStr">
-        <is>
-          <t>Johan Tamminen</t>
-        </is>
-      </c>
-      <c r="B108" s="11" t="inlineStr">
-        <is>
-          <t>Elli Tamminen</t>
-        </is>
-      </c>
-    </row>
-    <row r="109">
-      <c r="A109" s="6" t="inlineStr">
-        <is>
-          <t>Konsta Tamminen</t>
-        </is>
-      </c>
-      <c r="B109" s="11" t="inlineStr">
-        <is>
-          <t>Marja-Liisa Tamminen</t>
-        </is>
-      </c>
+      <c r="B109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr"/>
       <c r="B110" t="inlineStr"/>
     </row>
     <row r="111">
-      <c r="A111" t="inlineStr"/>
-      <c r="B111" s="2" t="inlineStr">
+      <c r="A111" s="3" t="inlineStr">
         <is>
           <t>a</t>
         </is>
       </c>
+      <c r="B111" s="4" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
     </row>
     <row r="112">
-      <c r="A112" s="3" t="inlineStr">
+      <c r="A112" s="11" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="B112" s="7" t="inlineStr">
         <is>
           <t>d</t>
         </is>
       </c>
-      <c r="B112" s="12" t="inlineStr">
-        <is>
-          <t>c</t>
-        </is>
-      </c>
     </row>
     <row r="113">
-      <c r="A113" s="7" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
-      </c>
+      <c r="A113" t="inlineStr"/>
       <c r="B113" t="inlineStr"/>
     </row>
     <row r="114">
-      <c r="A114" t="inlineStr"/>
+      <c r="A114" s="14" t="inlineStr">
+        <is>
+          <t>w</t>
+        </is>
+      </c>
       <c r="B114" t="inlineStr"/>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr"/>
+      <c r="B115" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>